<commit_message>
finished my design document
</commit_message>
<xml_diff>
--- a/Assessement1_itteration1/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/Assessement1_itteration1/ARA DATA Wait Lists Feb 2021.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="546" documentId="8_{1428531A-2172-4493-84B4-CAD89535E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5471A90F-1DCA-4E52-9866-35096C228DB2}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="4935" windowWidth="27135" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2010" windowWidth="27135" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -2760,8 +2760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" topLeftCell="I61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>